<commit_message>
intro, model, data in report
</commit_message>
<xml_diff>
--- a/Assignment 2/data_desc.xlsx
+++ b/Assignment 2/data_desc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data_desc" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -875,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>